<commit_message>
Authors as metadata import complete
</commit_message>
<xml_diff>
--- a/sites/all/modules/custom/ef_excel/ef-article-authors-normalised-and-unique.xlsx
+++ b/sites/all/modules/custom/ef_excel/ef-article-authors-normalised-and-unique.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="303" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="303" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="All EF Article Authors" sheetId="1" state="visible" r:id="rId2"/>
@@ -9819,7 +9819,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">roman, Ingrid</t>
     </r>
@@ -11574,7 +11573,7 @@
     <t>Rafa Towalski</t>
   </si>
   <si>
-    <t>Towalski, Rafał</t>
+    <t>Towalski, Rafal</t>
   </si>
   <si>
     <t>Dispute over trade union rights in soap manufacturer</t>
@@ -14953,7 +14952,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -14976,40 +14974,34 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF262626"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF5A5A5A"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -15246,10 +15238,10 @@
   </sheetPr>
   <dimension ref="A1:R1774"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A1140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F1158" activeCellId="0" sqref="F1158"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A1431" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C1452" activeCellId="0" sqref="C1452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -50773,8 +50765,8 @@
   </sheetPr>
   <dimension ref="A1:A1018"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D85" activeCellId="0" sqref="D85"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A887" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A899" activeCellId="0" sqref="A899"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>